<commit_message>
Modifications on .txt and .xlsx metadata files
</commit_message>
<xml_diff>
--- a/Data/Processed/02_Metadados_Behav-Analysis_Acoustic-Exp.xlsx
+++ b/Data/Processed/02_Metadados_Behav-Analysis_Acoustic-Exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\Mestrado\Projeto\Artigos\Experimento\BESocio\Article_behav-S.max_V03\Data\Processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFF3014-AC0D-4FD4-A2A4-B7EDD377D15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9A2BE9-733A-4752-854D-4E0F963FD9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15885" windowHeight="10635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -42,145 +42,166 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>Individual's sex (male or female)</t>
-  </si>
-  <si>
     <t>Treatment</t>
   </si>
   <si>
     <t>t_limp</t>
   </si>
   <si>
-    <t>Duration (s) of emission of the behavior "Autopreening"</t>
-  </si>
-  <si>
     <t>n_limb</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Bill cleaning"</t>
-  </si>
-  <si>
     <t>n_bat</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Flapping of wings"</t>
-  </si>
-  <si>
     <t>n_abeb</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Bill opening"</t>
-  </si>
-  <si>
     <t>n_trec</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Feather settling"</t>
-  </si>
-  <si>
     <t>n_and</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Walking on the perch"</t>
-  </si>
-  <si>
     <t>n_vooc</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Flight"</t>
-  </si>
-  <si>
     <t>n_pulp</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Jump between perches"</t>
-  </si>
-  <si>
     <t>n_darp</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Jumping laterally"</t>
-  </si>
-  <si>
     <t>t_com</t>
   </si>
   <si>
-    <t>Duration (s) of emission of the behavior "Eating"</t>
-  </si>
-  <si>
     <t>t_for</t>
   </si>
   <si>
-    <t>Duration (s) of emission of the behavior "Foragin"</t>
-  </si>
-  <si>
     <t>n_def</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Defecation"</t>
-  </si>
-  <si>
     <t>t_obs</t>
   </si>
   <si>
-    <t>Duration (s) of emission of the behavior "Vigilance"</t>
-  </si>
-  <si>
     <t>n_empg</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Perch in the cage"</t>
-  </si>
-  <si>
     <t>n_pulo</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Jump on the perch changing orientation"</t>
-  </si>
-  <si>
     <t>n_estp</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Stretching neck"</t>
-  </si>
-  <si>
     <t>t_cant</t>
   </si>
   <si>
-    <t>Duration (s) of emission of the behavior "Singing"</t>
-  </si>
-  <si>
     <t>n_vocc</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Call"</t>
-  </si>
-  <si>
     <t>t_rel</t>
   </si>
   <si>
-    <t>Duration (s) of emission of the behavior "Perching"</t>
-  </si>
-  <si>
     <t>n_conf</t>
   </si>
   <si>
-    <t>Frequency of emission of the behavior "Confrontation"</t>
-  </si>
-  <si>
-    <t>AttributeName</t>
-  </si>
-  <si>
-    <t>AttributeDefinition</t>
-  </si>
-  <si>
     <t>t_beb</t>
   </si>
   <si>
-    <t>Duration (s) of emission of the behavior "Drinking"</t>
-  </si>
-  <si>
     <t>Experimental treatment with different levels os acoustic information</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>attributeName</t>
+  </si>
+  <si>
+    <t>attributeDefinition</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>numberType</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>natural</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>Sex of individuals male or female</t>
+  </si>
+  <si>
+    <t>Duration (s) of emission of the behavior Autopreening</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Bill cleaning</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Flapping of wings</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Bill opening</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Feather settling</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Walking on the perch</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Flight</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Jump between perches</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Jumping laterally</t>
+  </si>
+  <si>
+    <t>Duration (s) of emission of the behavior Eating</t>
+  </si>
+  <si>
+    <t>Duration (s) of emission of the behavior Foragin</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Defecation</t>
+  </si>
+  <si>
+    <t>Duration (s) of emission of the behavior Drinking</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Perch in the cage</t>
+  </si>
+  <si>
+    <t>Duration (s) of emission of the behavior Vigilance</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Jump on the perch changing orientation</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Stretching neck</t>
+  </si>
+  <si>
+    <t>Duration (s) of emission of the behavior Singing</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Call</t>
+  </si>
+  <si>
+    <t>Duration (s) of emission of the behavior Perching</t>
+  </si>
+  <si>
+    <t>Frequency of emission of the behavior Confrontation</t>
   </si>
 </sst>
 </file>
@@ -498,224 +519,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>